<commit_message>
CNY Updates - submit form
left the image submit
</commit_message>
<xml_diff>
--- a/Postsubmission_details.xlsx
+++ b/Postsubmission_details.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23515"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="3060" yWindow="780" windowWidth="38400" windowHeight="20140" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14600" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="17">
   <si>
     <t>Collection name</t>
   </si>
@@ -63,10 +63,13 @@
     <t>num</t>
   </si>
   <si>
-    <t>itemOriginalPrice</t>
-  </si>
-  <si>
     <t>itemLoves</t>
+  </si>
+  <si>
+    <t>userId</t>
+  </si>
+  <si>
+    <t>itemPrice</t>
   </si>
 </sst>
 </file>
@@ -98,12 +101,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -115,7 +124,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="17">
+  <cellStyleXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -133,11 +142,14 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="17">
+  <cellStyles count="19">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -146,6 +158,7 @@
     <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -154,6 +167,7 @@
     <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -526,10 +540,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="G6:I31"/>
+  <dimension ref="G6:I34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="I31" sqref="I31"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="M27" sqref="M27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -560,7 +574,7 @@
       <c r="G9">
         <v>2</v>
       </c>
-      <c r="H9" t="s">
+      <c r="H9" s="1" t="s">
         <v>0</v>
       </c>
       <c r="I9" t="s">
@@ -579,7 +593,7 @@
       <c r="G12">
         <v>3</v>
       </c>
-      <c r="H12" t="s">
+      <c r="H12" s="1" t="s">
         <v>0</v>
       </c>
       <c r="I12" t="s">
@@ -598,7 +612,7 @@
       <c r="G15">
         <v>4</v>
       </c>
-      <c r="H15" t="s">
+      <c r="H15" s="1" t="s">
         <v>0</v>
       </c>
       <c r="I15" t="s">
@@ -617,7 +631,7 @@
       <c r="G18">
         <v>5</v>
       </c>
-      <c r="H18" t="s">
+      <c r="H18" s="1" t="s">
         <v>0</v>
       </c>
       <c r="I18" t="s">
@@ -674,11 +688,11 @@
       <c r="G27">
         <v>8</v>
       </c>
-      <c r="H27" t="s">
+      <c r="H27" s="1" t="s">
         <v>0</v>
       </c>
       <c r="I27" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="28" spans="7:9">
@@ -693,11 +707,11 @@
       <c r="G30">
         <v>9</v>
       </c>
-      <c r="H30" t="s">
+      <c r="H30" s="1" t="s">
         <v>0</v>
       </c>
       <c r="I30" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="31" spans="7:9">
@@ -706,6 +720,22 @@
       </c>
       <c r="I31" t="s">
         <v>13</v>
+      </c>
+    </row>
+    <row r="33" spans="8:9">
+      <c r="H33" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I33" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="34" spans="8:9">
+      <c r="H34" t="s">
+        <v>2</v>
+      </c>
+      <c r="I34" t="s">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>